<commit_message>
deep refactor, in progress..
</commit_message>
<xml_diff>
--- a/src/samples/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
+++ b/src/samples/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
@@ -420,18 +420,18 @@
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="n5nz24iu" xfId="1"/>
-    <cellStyle name="n5nz24iu_Alternate" xfId="2"/>
-    <cellStyle name="wqj1ijzm" xfId="3"/>
-    <cellStyle name="wqj1ijzm_Alternate" xfId="4"/>
-    <cellStyle name="htbpa13u" xfId="5"/>
-    <cellStyle name="htbpa13u_Alternate" xfId="6"/>
-    <cellStyle name="0prl0ula" xfId="7"/>
-    <cellStyle name="0prl0ula_Alternate" xfId="8"/>
-    <cellStyle name="4nbh1ut0" xfId="9"/>
-    <cellStyle name="4nbh1ut0_Alternate" xfId="10"/>
-    <cellStyle name="2mmoazj3" xfId="11"/>
-    <cellStyle name="2mmoazj3_Alternate" xfId="12"/>
+    <cellStyle name="2c0mgcci" xfId="1"/>
+    <cellStyle name="2c0mgcci_Alternate" xfId="2"/>
+    <cellStyle name="nosdlcql" xfId="3"/>
+    <cellStyle name="nosdlcql_Alternate" xfId="4"/>
+    <cellStyle name="5pe5ks0t" xfId="5"/>
+    <cellStyle name="5pe5ks0t_Alternate" xfId="6"/>
+    <cellStyle name="tnzlcq2u" xfId="7"/>
+    <cellStyle name="tnzlcq2u_Alternate" xfId="8"/>
+    <cellStyle name="xfjyyyx1" xfId="9"/>
+    <cellStyle name="xfjyyyx1_Alternate" xfId="10"/>
+    <cellStyle name="glueig0l" xfId="11"/>
+    <cellStyle name="glueig0l_Alternate" xfId="12"/>
     <cellStyle name="LocalHeader-1" xfId="13"/>
     <cellStyle name="LocalHeader-1_Alternate" xfId="14"/>
     <cellStyle name="LocalHeader0" xfId="15"/>
@@ -450,10 +450,10 @@
     <cellStyle name="LocalHeader6_Alternate" xfId="28"/>
     <cellStyle name="LocalHeader7" xfId="29"/>
     <cellStyle name="LocalHeader7_Alternate" xfId="30"/>
-    <cellStyle name="axk0eiu4" xfId="31"/>
-    <cellStyle name="axk0eiu4_Alternate" xfId="32"/>
-    <cellStyle name="afylztfl" xfId="33"/>
-    <cellStyle name="afylztfl_Alternate" xfId="34"/>
+    <cellStyle name="ogxritj2" xfId="31"/>
+    <cellStyle name="ogxritj2_Alternate" xfId="32"/>
+    <cellStyle name="35mr4tr2" xfId="33"/>
+    <cellStyle name="35mr4tr2_Alternate" xfId="34"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>

</xml_diff>

<commit_message>
refactor in solution, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
+++ b/src/samples/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Informe test</t>
   </si>
@@ -45,7 +45,13 @@
     <t>Fecha Inicio</t>
   </si>
   <si>
+    <t>01/01/2019 0:00:00</t>
+  </si>
+  <si>
     <t>Fecha Fin</t>
+  </si>
+  <si>
+    <t>10/07/2020 0:00:00</t>
   </si>
   <si>
     <t>APOLO HOTEL</t>
@@ -79,11 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00;[Black]\-#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0;[Black]\-#,##0.0"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -228,22 +230,22 @@
     <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1">
@@ -300,16 +302,16 @@
     <xf numFmtId="49" fontId="4" fillId="10" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0">
+    <xf numFmtId="49" fontId="3" fillId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="1">
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="1">
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -333,22 +335,22 @@
     <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="6" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="7" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="8" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="8" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="9" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="9" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="10" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="10" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="11" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="11" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="13" applyProtection="1" applyAlignment="1">
@@ -405,33 +407,33 @@
     <xf numFmtId="49" applyNumberFormat="1" fontId="4" applyFont="1" fillId="10" applyFill="1" borderId="1" applyBorder="1" xfId="30" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="31" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="31" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="32" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" xfId="32" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="1" applyBorder="1" xfId="33" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="1" applyBorder="1" xfId="33" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="1" applyBorder="1" xfId="34" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="1" applyBorder="1" xfId="34" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="2c0mgcci" xfId="1"/>
-    <cellStyle name="2c0mgcci_Alternate" xfId="2"/>
-    <cellStyle name="nosdlcql" xfId="3"/>
-    <cellStyle name="nosdlcql_Alternate" xfId="4"/>
-    <cellStyle name="5pe5ks0t" xfId="5"/>
-    <cellStyle name="5pe5ks0t_Alternate" xfId="6"/>
-    <cellStyle name="tnzlcq2u" xfId="7"/>
-    <cellStyle name="tnzlcq2u_Alternate" xfId="8"/>
-    <cellStyle name="xfjyyyx1" xfId="9"/>
-    <cellStyle name="xfjyyyx1_Alternate" xfId="10"/>
-    <cellStyle name="glueig0l" xfId="11"/>
-    <cellStyle name="glueig0l_Alternate" xfId="12"/>
+    <cellStyle name="zmjiw50i" xfId="1"/>
+    <cellStyle name="zmjiw50i_Alternate" xfId="2"/>
+    <cellStyle name="ze0241vf" xfId="3"/>
+    <cellStyle name="ze0241vf_Alternate" xfId="4"/>
+    <cellStyle name="tyxxlc2b" xfId="5"/>
+    <cellStyle name="tyxxlc2b_Alternate" xfId="6"/>
+    <cellStyle name="ozfk3nd1" xfId="7"/>
+    <cellStyle name="ozfk3nd1_Alternate" xfId="8"/>
+    <cellStyle name="acaet2li" xfId="9"/>
+    <cellStyle name="acaet2li_Alternate" xfId="10"/>
+    <cellStyle name="2i4ll2bt" xfId="11"/>
+    <cellStyle name="2i4ll2bt_Alternate" xfId="12"/>
     <cellStyle name="LocalHeader-1" xfId="13"/>
     <cellStyle name="LocalHeader-1_Alternate" xfId="14"/>
     <cellStyle name="LocalHeader0" xfId="15"/>
@@ -450,10 +452,10 @@
     <cellStyle name="LocalHeader6_Alternate" xfId="28"/>
     <cellStyle name="LocalHeader7" xfId="29"/>
     <cellStyle name="LocalHeader7_Alternate" xfId="30"/>
-    <cellStyle name="ogxritj2" xfId="31"/>
-    <cellStyle name="ogxritj2_Alternate" xfId="32"/>
-    <cellStyle name="35mr4tr2" xfId="33"/>
-    <cellStyle name="35mr4tr2_Alternate" xfId="34"/>
+    <cellStyle name="r4es4t05" xfId="31"/>
+    <cellStyle name="r4es4t05_Alternate" xfId="32"/>
+    <cellStyle name="34jafted" xfId="33"/>
+    <cellStyle name="34jafted_Alternate" xfId="34"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -507,16 +509,16 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
-        <v>43466</v>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8">
-        <v>44022</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -537,7 +539,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="1" width="13.113714218139648" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="10.140625" customWidth="1"/>
     <col min="3" max="3" bestFit="1" width="15.64161491394043" customWidth="1"/>
     <col min="4" max="4" bestFit="1" width="15.325394630432129" customWidth="1"/>
     <col min="5" max="5" bestFit="1" width="18.184396743774414" customWidth="1"/>
@@ -551,31 +553,31 @@
   <sheetData>
     <row r="2">
       <c r="C2" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -18578,568 +18580,568 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" bestFit="1" width="34.549720764160156" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="10" max="10" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="11" max="11" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="12" max="12" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="13" max="13" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="14" max="14" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="15" max="15" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="16" max="16" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="17" max="17" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="18" max="18" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="19" max="19" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="20" max="20" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="21" max="21" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="22" max="22" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="23" max="23" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="24" max="24" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="25" max="25" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="26" max="26" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="27" max="27" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="28" max="28" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="29" max="29" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="30" max="30" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="31" max="31" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="32" max="32" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="33" max="33" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="34" max="34" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="35" max="35" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="36" max="36" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="37" max="37" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="38" max="38" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="39" max="39" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="40" max="40" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="41" max="41" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="42" max="42" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="43" max="43" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="44" max="44" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="45" max="45" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="46" max="46" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="47" max="47" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="48" max="48" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="49" max="49" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="50" max="50" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="51" max="51" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="52" max="52" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="53" max="53" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="54" max="54" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="55" max="55" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="56" max="56" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="57" max="57" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="58" max="58" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="59" max="59" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="60" max="60" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="61" max="61" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="62" max="62" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="63" max="63" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="64" max="64" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="65" max="65" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="66" max="66" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="67" max="67" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="68" max="68" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="69" max="69" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="70" max="70" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="71" max="71" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="72" max="72" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="73" max="73" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="74" max="74" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="75" max="75" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="76" max="76" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="77" max="77" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="78" max="78" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="79" max="79" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="80" max="80" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="81" max="81" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="82" max="82" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="83" max="83" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="84" max="84" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="85" max="85" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="86" max="86" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="87" max="87" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="88" max="88" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="89" max="89" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="90" max="90" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="91" max="91" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="92" max="92" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="93" max="93" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="94" max="94" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="95" max="95" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="96" max="96" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="97" max="97" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="98" max="98" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="99" max="99" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="100" max="100" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="101" max="101" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="102" max="102" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="103" max="103" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="104" max="104" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="105" max="105" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="106" max="106" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="107" max="107" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="108" max="108" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="109" max="109" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="110" max="110" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="111" max="111" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="112" max="112" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="113" max="113" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="114" max="114" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="115" max="115" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="116" max="116" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="117" max="117" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="118" max="118" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="119" max="119" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="120" max="120" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="121" max="121" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="122" max="122" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="123" max="123" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="124" max="124" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="125" max="125" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="126" max="126" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="127" max="127" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="128" max="128" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="129" max="129" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="130" max="130" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="131" max="131" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="132" max="132" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="133" max="133" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="134" max="134" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="135" max="135" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="136" max="136" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="137" max="137" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="138" max="138" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="139" max="139" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="140" max="140" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="141" max="141" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="142" max="142" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="143" max="143" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="144" max="144" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="145" max="145" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="146" max="146" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="147" max="147" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="148" max="148" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="149" max="149" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="150" max="150" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="151" max="151" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="152" max="152" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="153" max="153" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="154" max="154" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="155" max="155" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="156" max="156" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="157" max="157" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="158" max="158" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="159" max="159" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="160" max="160" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="161" max="161" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="162" max="162" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="163" max="163" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="164" max="164" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="165" max="165" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="166" max="166" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="167" max="167" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="168" max="168" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="169" max="169" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="170" max="170" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="171" max="171" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="172" max="172" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="173" max="173" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="174" max="174" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="175" max="175" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="176" max="176" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="177" max="177" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="178" max="178" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="179" max="179" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="180" max="180" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="181" max="181" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="182" max="182" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="183" max="183" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="184" max="184" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="185" max="185" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="186" max="186" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="187" max="187" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="188" max="188" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="189" max="189" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="190" max="190" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="191" max="191" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="192" max="192" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="193" max="193" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="194" max="194" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="195" max="195" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="196" max="196" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="197" max="197" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="198" max="198" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="199" max="199" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="200" max="200" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="201" max="201" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="202" max="202" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="203" max="203" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="204" max="204" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="205" max="205" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="206" max="206" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="207" max="207" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="208" max="208" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="209" max="209" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="210" max="210" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="211" max="211" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="212" max="212" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="213" max="213" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="214" max="214" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="215" max="215" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="216" max="216" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="217" max="217" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="218" max="218" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="219" max="219" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="220" max="220" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="221" max="221" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="222" max="222" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="223" max="223" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="224" max="224" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="225" max="225" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="226" max="226" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="227" max="227" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="228" max="228" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="229" max="229" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="230" max="230" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="231" max="231" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="232" max="232" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="233" max="233" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="234" max="234" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="235" max="235" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="236" max="236" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="237" max="237" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="238" max="238" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="239" max="239" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="240" max="240" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="241" max="241" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="242" max="242" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="243" max="243" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="244" max="244" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="245" max="245" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="246" max="246" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="247" max="247" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="248" max="248" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="249" max="249" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="250" max="250" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="251" max="251" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="252" max="252" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="253" max="253" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="254" max="254" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="255" max="255" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="256" max="256" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="257" max="257" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="258" max="258" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="259" max="259" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="260" max="260" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="261" max="261" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="262" max="262" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="263" max="263" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="264" max="264" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="265" max="265" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="266" max="266" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="267" max="267" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="268" max="268" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="269" max="269" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="270" max="270" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="271" max="271" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="272" max="272" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="273" max="273" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="274" max="274" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="275" max="275" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="276" max="276" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="277" max="277" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="278" max="278" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="279" max="279" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="280" max="280" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="281" max="281" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="282" max="282" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="283" max="283" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="284" max="284" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="285" max="285" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="286" max="286" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="287" max="287" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="288" max="288" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="289" max="289" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="290" max="290" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="291" max="291" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="292" max="292" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="293" max="293" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="294" max="294" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="295" max="295" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="296" max="296" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="297" max="297" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="298" max="298" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="299" max="299" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="300" max="300" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="301" max="301" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="302" max="302" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="303" max="303" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="304" max="304" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="305" max="305" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="306" max="306" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="307" max="307" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="308" max="308" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="309" max="309" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="310" max="310" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="311" max="311" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="312" max="312" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="313" max="313" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="314" max="314" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="315" max="315" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="316" max="316" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="317" max="317" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="318" max="318" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="319" max="319" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="320" max="320" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="321" max="321" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="322" max="322" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="323" max="323" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="324" max="324" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="325" max="325" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="326" max="326" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="327" max="327" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="328" max="328" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="329" max="329" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="330" max="330" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="331" max="331" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="332" max="332" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="333" max="333" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="334" max="334" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="335" max="335" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="336" max="336" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="337" max="337" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="338" max="338" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="339" max="339" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="340" max="340" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="341" max="341" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="342" max="342" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="343" max="343" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="344" max="344" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="345" max="345" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="346" max="346" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="347" max="347" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="348" max="348" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="349" max="349" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="350" max="350" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="351" max="351" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="352" max="352" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="353" max="353" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="354" max="354" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="355" max="355" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="356" max="356" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="357" max="357" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="358" max="358" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="359" max="359" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="360" max="360" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="361" max="361" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="362" max="362" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="363" max="363" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="364" max="364" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="365" max="365" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="366" max="366" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="367" max="367" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="368" max="368" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="369" max="369" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="370" max="370" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="371" max="371" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="372" max="372" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="373" max="373" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="374" max="374" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="375" max="375" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="376" max="376" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="377" max="377" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="378" max="378" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="379" max="379" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="380" max="380" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="381" max="381" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="382" max="382" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="383" max="383" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="384" max="384" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="385" max="385" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="386" max="386" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="387" max="387" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="388" max="388" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="389" max="389" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="390" max="390" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="391" max="391" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="392" max="392" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="393" max="393" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="394" max="394" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="395" max="395" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="396" max="396" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="397" max="397" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="398" max="398" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="399" max="399" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="400" max="400" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="401" max="401" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="402" max="402" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="403" max="403" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="404" max="404" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="405" max="405" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="406" max="406" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="407" max="407" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="408" max="408" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="409" max="409" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="410" max="410" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="411" max="411" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="412" max="412" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="413" max="413" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="414" max="414" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="415" max="415" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="416" max="416" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="417" max="417" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="418" max="418" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="419" max="419" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="420" max="420" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="421" max="421" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="422" max="422" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="423" max="423" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="424" max="424" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="425" max="425" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="426" max="426" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="427" max="427" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="428" max="428" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="429" max="429" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="430" max="430" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="431" max="431" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="432" max="432" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="433" max="433" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="434" max="434" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="435" max="435" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="436" max="436" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="437" max="437" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="438" max="438" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="439" max="439" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="440" max="440" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="441" max="441" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="442" max="442" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="443" max="443" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="444" max="444" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="445" max="445" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="446" max="446" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="447" max="447" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="448" max="448" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="449" max="449" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="450" max="450" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="451" max="451" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="452" max="452" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="453" max="453" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="454" max="454" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="455" max="455" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="456" max="456" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="457" max="457" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="458" max="458" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="459" max="459" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="460" max="460" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="461" max="461" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="462" max="462" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="463" max="463" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="464" max="464" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="465" max="465" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="466" max="466" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="467" max="467" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="468" max="468" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="469" max="469" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="470" max="470" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="471" max="471" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="472" max="472" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="473" max="473" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="474" max="474" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="475" max="475" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="476" max="476" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="477" max="477" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="478" max="478" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="479" max="479" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="480" max="480" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="481" max="481" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="482" max="482" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="483" max="483" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="484" max="484" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="485" max="485" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="486" max="486" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="487" max="487" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="488" max="488" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="489" max="489" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="490" max="490" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="491" max="491" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="492" max="492" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="493" max="493" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="494" max="494" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="495" max="495" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="496" max="496" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="497" max="497" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="498" max="498" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="499" max="499" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="500" max="500" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="501" max="501" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="502" max="502" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="503" max="503" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="504" max="504" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="505" max="505" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="506" max="506" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="507" max="507" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="508" max="508" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="509" max="509" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="510" max="510" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="511" max="511" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="512" max="512" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="513" max="513" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="514" max="514" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="515" max="515" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="516" max="516" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="517" max="517" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="518" max="518" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="519" max="519" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="520" max="520" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="521" max="521" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="522" max="522" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="523" max="523" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="524" max="524" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="525" max="525" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="526" max="526" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="527" max="527" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="528" max="528" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="529" max="529" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="530" max="530" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="531" max="531" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="532" max="532" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="533" max="533" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="534" max="534" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="535" max="535" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="536" max="536" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="537" max="537" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="538" max="538" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="539" max="539" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="540" max="540" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="541" max="541" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="542" max="542" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="543" max="543" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="544" max="544" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="545" max="545" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="546" max="546" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="547" max="547" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="548" max="548" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="549" max="549" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="550" max="550" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="551" max="551" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="552" max="552" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="553" max="553" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="554" max="554" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="555" max="555" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="556" max="556" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="557" max="557" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="558" max="558" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="559" max="559" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="560" max="560" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="561" max="561" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="562" max="562" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="563" max="563" bestFit="1" width="13.113714218139648" customWidth="1"/>
-    <col min="564" max="564" bestFit="1" width="13.113714218139648" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="18" max="18" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="20" max="20" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="21" max="21" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="22" max="22" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="24" max="24" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="25" max="25" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="27" max="27" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="28" max="28" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="29" max="29" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="30" max="30" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="31" max="31" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="33" max="33" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="34" max="34" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="35" max="35" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="36" max="36" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="37" max="37" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="38" max="38" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="39" max="39" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="40" max="40" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="41" max="41" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="42" max="42" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="43" max="43" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="44" max="44" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="45" max="45" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="46" max="46" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="47" max="47" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="48" max="48" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="49" max="49" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="50" max="50" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="51" max="51" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="52" max="52" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="53" max="53" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="54" max="54" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="55" max="55" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="56" max="56" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="57" max="57" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="58" max="58" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="59" max="59" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="60" max="60" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="61" max="61" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="62" max="62" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="63" max="63" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="64" max="64" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="65" max="65" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="66" max="66" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="67" max="67" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="68" max="68" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="69" max="69" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="70" max="70" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="71" max="71" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="72" max="72" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="73" max="73" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="74" max="74" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="75" max="75" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="76" max="76" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="77" max="77" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="78" max="78" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="79" max="79" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="80" max="80" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="81" max="81" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="82" max="82" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="83" max="83" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="84" max="84" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="85" max="85" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="86" max="86" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="87" max="87" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="88" max="88" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="89" max="89" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="90" max="90" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="91" max="91" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="92" max="92" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="93" max="93" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="94" max="94" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="95" max="95" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="96" max="96" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="97" max="97" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="98" max="98" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="99" max="99" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="100" max="100" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="101" max="101" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="102" max="102" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="103" max="103" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="104" max="104" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="105" max="105" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="106" max="106" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="107" max="107" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="108" max="108" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="109" max="109" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="110" max="110" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="111" max="111" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="112" max="112" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="113" max="113" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="114" max="114" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="115" max="115" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="116" max="116" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="117" max="117" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="118" max="118" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="119" max="119" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="120" max="120" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="121" max="121" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="122" max="122" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="123" max="123" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="124" max="124" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="125" max="125" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="126" max="126" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="127" max="127" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="128" max="128" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="129" max="129" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="130" max="130" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="131" max="131" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="132" max="132" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="133" max="133" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="134" max="134" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="135" max="135" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="136" max="136" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="137" max="137" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="138" max="138" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="139" max="139" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="140" max="140" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="141" max="141" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="142" max="142" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="143" max="143" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="144" max="144" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="145" max="145" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="146" max="146" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="147" max="147" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="148" max="148" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="149" max="149" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="150" max="150" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="151" max="151" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="152" max="152" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="153" max="153" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="154" max="154" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="155" max="155" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="156" max="156" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="157" max="157" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="158" max="158" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="159" max="159" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="160" max="160" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="161" max="161" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="162" max="162" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="163" max="163" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="164" max="164" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="165" max="165" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="166" max="166" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="167" max="167" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="168" max="168" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="169" max="169" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="170" max="170" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="171" max="171" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="172" max="172" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="173" max="173" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="174" max="174" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="175" max="175" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="176" max="176" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="177" max="177" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="178" max="178" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="179" max="179" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="180" max="180" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="181" max="181" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="182" max="182" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="183" max="183" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="184" max="184" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="185" max="185" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="186" max="186" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="187" max="187" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="188" max="188" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="189" max="189" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="190" max="190" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="191" max="191" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="192" max="192" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="193" max="193" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="194" max="194" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="195" max="195" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="196" max="196" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="197" max="197" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="198" max="198" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="199" max="199" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="200" max="200" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="201" max="201" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="202" max="202" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="203" max="203" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="204" max="204" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="205" max="205" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="206" max="206" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="207" max="207" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="208" max="208" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="209" max="209" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="210" max="210" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="211" max="211" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="212" max="212" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="213" max="213" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="214" max="214" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="215" max="215" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="216" max="216" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="217" max="217" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="218" max="218" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="219" max="219" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="220" max="220" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="221" max="221" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="222" max="222" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="223" max="223" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="224" max="224" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="225" max="225" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="226" max="226" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="227" max="227" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="228" max="228" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="229" max="229" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="230" max="230" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="231" max="231" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="232" max="232" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="233" max="233" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="234" max="234" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="235" max="235" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="236" max="236" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="237" max="237" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="238" max="238" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="239" max="239" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="240" max="240" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="241" max="241" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="242" max="242" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="243" max="243" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="244" max="244" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="245" max="245" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="246" max="246" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="247" max="247" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="248" max="248" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="249" max="249" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="250" max="250" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="251" max="251" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="252" max="252" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="253" max="253" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="254" max="254" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="255" max="255" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="256" max="256" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="257" max="257" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="258" max="258" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="259" max="259" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="260" max="260" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="261" max="261" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="262" max="262" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="263" max="263" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="264" max="264" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="265" max="265" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="266" max="266" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="267" max="267" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="268" max="268" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="269" max="269" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="270" max="270" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="271" max="271" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="272" max="272" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="273" max="273" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="274" max="274" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="275" max="275" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="276" max="276" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="277" max="277" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="278" max="278" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="279" max="279" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="280" max="280" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="281" max="281" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="282" max="282" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="283" max="283" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="284" max="284" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="285" max="285" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="286" max="286" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="287" max="287" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="288" max="288" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="289" max="289" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="290" max="290" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="291" max="291" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="292" max="292" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="293" max="293" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="294" max="294" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="295" max="295" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="296" max="296" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="297" max="297" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="298" max="298" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="299" max="299" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="300" max="300" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="301" max="301" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="302" max="302" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="303" max="303" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="304" max="304" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="305" max="305" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="306" max="306" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="307" max="307" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="308" max="308" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="309" max="309" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="310" max="310" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="311" max="311" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="312" max="312" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="313" max="313" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="314" max="314" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="315" max="315" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="316" max="316" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="317" max="317" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="318" max="318" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="319" max="319" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="320" max="320" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="321" max="321" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="322" max="322" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="323" max="323" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="324" max="324" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="325" max="325" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="326" max="326" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="327" max="327" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="328" max="328" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="329" max="329" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="330" max="330" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="331" max="331" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="332" max="332" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="333" max="333" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="334" max="334" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="335" max="335" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="336" max="336" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="337" max="337" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="338" max="338" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="339" max="339" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="340" max="340" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="341" max="341" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="342" max="342" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="343" max="343" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="344" max="344" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="345" max="345" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="346" max="346" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="347" max="347" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="348" max="348" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="349" max="349" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="350" max="350" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="351" max="351" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="352" max="352" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="353" max="353" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="354" max="354" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="355" max="355" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="356" max="356" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="357" max="357" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="358" max="358" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="359" max="359" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="360" max="360" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="361" max="361" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="362" max="362" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="363" max="363" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="364" max="364" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="365" max="365" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="366" max="366" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="367" max="367" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="368" max="368" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="369" max="369" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="370" max="370" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="371" max="371" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="372" max="372" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="373" max="373" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="374" max="374" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="375" max="375" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="376" max="376" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="377" max="377" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="378" max="378" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="379" max="379" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="380" max="380" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="381" max="381" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="382" max="382" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="383" max="383" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="384" max="384" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="385" max="385" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="386" max="386" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="387" max="387" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="388" max="388" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="389" max="389" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="390" max="390" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="391" max="391" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="392" max="392" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="393" max="393" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="394" max="394" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="395" max="395" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="396" max="396" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="397" max="397" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="398" max="398" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="399" max="399" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="400" max="400" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="401" max="401" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="402" max="402" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="403" max="403" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="404" max="404" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="405" max="405" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="406" max="406" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="407" max="407" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="408" max="408" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="409" max="409" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="410" max="410" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="411" max="411" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="412" max="412" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="413" max="413" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="414" max="414" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="415" max="415" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="416" max="416" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="417" max="417" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="418" max="418" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="419" max="419" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="420" max="420" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="421" max="421" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="422" max="422" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="423" max="423" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="424" max="424" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="425" max="425" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="426" max="426" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="427" max="427" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="428" max="428" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="429" max="429" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="430" max="430" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="431" max="431" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="432" max="432" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="433" max="433" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="434" max="434" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="435" max="435" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="436" max="436" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="437" max="437" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="438" max="438" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="439" max="439" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="440" max="440" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="441" max="441" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="442" max="442" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="443" max="443" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="444" max="444" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="445" max="445" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="446" max="446" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="447" max="447" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="448" max="448" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="449" max="449" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="450" max="450" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="451" max="451" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="452" max="452" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="453" max="453" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="454" max="454" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="455" max="455" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="456" max="456" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="457" max="457" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="458" max="458" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="459" max="459" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="460" max="460" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="461" max="461" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="462" max="462" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="463" max="463" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="464" max="464" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="465" max="465" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="466" max="466" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="467" max="467" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="468" max="468" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="469" max="469" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="470" max="470" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="471" max="471" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="472" max="472" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="473" max="473" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="474" max="474" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="475" max="475" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="476" max="476" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="477" max="477" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="478" max="478" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="479" max="479" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="480" max="480" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="481" max="481" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="482" max="482" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="483" max="483" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="484" max="484" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="485" max="485" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="486" max="486" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="487" max="487" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="488" max="488" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="489" max="489" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="490" max="490" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="491" max="491" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="492" max="492" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="493" max="493" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="494" max="494" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="495" max="495" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="496" max="496" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="497" max="497" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="498" max="498" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="499" max="499" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="500" max="500" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="501" max="501" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="502" max="502" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="503" max="503" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="504" max="504" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="505" max="505" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="506" max="506" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="507" max="507" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="508" max="508" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="509" max="509" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="510" max="510" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="511" max="511" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="512" max="512" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="513" max="513" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="514" max="514" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="515" max="515" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="516" max="516" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="517" max="517" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="518" max="518" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="519" max="519" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="520" max="520" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="521" max="521" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="522" max="522" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="523" max="523" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="524" max="524" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="525" max="525" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="526" max="526" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="527" max="527" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="528" max="528" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="529" max="529" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="530" max="530" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="531" max="531" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="532" max="532" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="533" max="533" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="534" max="534" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="535" max="535" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="536" max="536" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="537" max="537" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="538" max="538" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="539" max="539" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="540" max="540" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="541" max="541" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="542" max="542" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="543" max="543" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="544" max="544" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="545" max="545" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="546" max="546" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="547" max="547" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="548" max="548" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="549" max="549" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="550" max="550" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="551" max="551" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="552" max="552" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="553" max="553" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="554" max="554" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="555" max="555" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="556" max="556" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="557" max="557" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="558" max="558" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="559" max="559" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="560" max="560" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="561" max="561" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="562" max="562" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="563" max="563" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="564" max="564" bestFit="1" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -20832,7 +20834,7 @@
     </row>
     <row r="4">
       <c r="B4" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
@@ -22523,7 +22525,7 @@
     </row>
     <row r="5">
       <c r="B5" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="31">
         <v>0</v>
@@ -24214,7 +24216,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" s="31">
         <v>0</v>
@@ -25905,7 +25907,7 @@
     </row>
     <row r="7">
       <c r="B7" s="20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="31">
         <v>6</v>
@@ -27596,7 +27598,7 @@
     </row>
     <row r="8">
       <c r="B8" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="31">
         <v>0</v>
@@ -29287,7 +29289,7 @@
     </row>
     <row r="9">
       <c r="B9" s="24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="31">
         <v>1</v>
@@ -30978,7 +30980,7 @@
     </row>
     <row r="10">
       <c r="B10" s="25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="31">
         <v>0</v>
@@ -32669,7 +32671,7 @@
     </row>
     <row r="11">
       <c r="B11" s="28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="31">
         <v>1</v>
@@ -34360,7 +34362,7 @@
     </row>
     <row r="12">
       <c r="B12" s="29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="31">
         <v>1.125</v>

</xml_diff>